<commit_message>
21/9/9 modify in the afternoon
</commit_message>
<xml_diff>
--- a/UNIX网络编程/Unix Network V1阅读/UNIX Network Programming, Volume 1阅读计划.xlsx
+++ b/UNIX网络编程/Unix Network V1阅读/UNIX Network Programming, Volume 1阅读计划.xlsx
@@ -1165,8 +1165,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
@@ -1191,6 +1191,28 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -1205,6 +1227,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -1212,29 +1241,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1248,6 +1255,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -1256,8 +1271,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -1289,23 +1311,8 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1313,14 +1320,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1355,19 +1355,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1385,7 +1385,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1397,19 +1415,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1427,31 +1493,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1463,79 +1535,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1546,6 +1546,30 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1564,17 +1588,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1603,35 +1621,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1654,10 +1654,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1666,133 +1666,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2162,8 +2162,8 @@
   <sheetPr/>
   <dimension ref="A1:C368"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A268" workbookViewId="0">
-      <selection activeCell="B232" sqref="B232"/>
+    <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
+      <selection activeCell="C201" sqref="C201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="2"/>
@@ -4242,12 +4242,15 @@
     <row r="199" spans="1:1">
       <c r="A199" s="1"/>
     </row>
-    <row r="200" spans="1:2">
+    <row r="200" spans="1:3">
       <c r="A200" s="1" t="s">
         <v>186</v>
       </c>
       <c r="B200" s="2">
         <v>44434</v>
+      </c>
+      <c r="C200" s="2">
+        <v>44448</v>
       </c>
     </row>
     <row r="201" spans="1:2">

</xml_diff>